<commit_message>
Updated codebook and spreadsheet
Updated codebook and spreadsheet to reflect changes in column names, updated counts, etc.
</commit_message>
<xml_diff>
--- a/reports/Data Dictionary_Codebook.xlsx
+++ b/reports/Data Dictionary_Codebook.xlsx
@@ -166,7 +166,7 @@
     <t>ACS_PCT_HU_MOBILE_HOME</t>
   </si>
   <si>
-    <t>Pct_mobil_homes</t>
+    <t>Pct_mobile_homes</t>
   </si>
   <si>
     <t>Percentage of housing units that are mobile homes</t>
@@ -1192,7 +1192,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H48" displayName="Table1" name="Table1" id="1">
-  <autoFilter ref="$A$1:$H$48"/>
+  <autoFilter ref="$A$1:$H$48">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Y"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="8">
     <tableColumn name="Variable" id="1"/>
     <tableColumn name="Renamed Variable" id="2"/>
@@ -1501,7 +1507,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" hidden="1">
       <c r="A4" s="6" t="s">
         <v>21</v>
       </c>
@@ -1579,7 +1585,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" hidden="1">
       <c r="A7" s="11" t="s">
         <v>36</v>
       </c>
@@ -1605,7 +1611,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" hidden="1">
       <c r="A8" s="6" t="s">
         <v>40</v>
       </c>
@@ -1683,7 +1689,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" hidden="1">
       <c r="A11" s="11" t="s">
         <v>53</v>
       </c>
@@ -1709,7 +1715,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" hidden="1">
       <c r="A12" s="6" t="s">
         <v>58</v>
       </c>
@@ -1735,7 +1741,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" hidden="1">
       <c r="A13" s="11" t="s">
         <v>63</v>
       </c>
@@ -1787,7 +1793,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" hidden="1">
       <c r="A15" s="11" t="s">
         <v>71</v>
       </c>
@@ -1813,7 +1819,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" hidden="1">
       <c r="A16" s="6" t="s">
         <v>75</v>
       </c>
@@ -1839,7 +1845,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" hidden="1">
       <c r="A17" s="11" t="s">
         <v>79</v>
       </c>
@@ -1865,7 +1871,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" hidden="1">
       <c r="A18" s="6" t="s">
         <v>83</v>
       </c>
@@ -1891,7 +1897,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" hidden="1">
       <c r="A19" s="11" t="s">
         <v>87</v>
       </c>
@@ -1917,7 +1923,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" hidden="1">
       <c r="A20" s="6" t="s">
         <v>91</v>
       </c>
@@ -2021,7 +2027,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" hidden="1">
       <c r="A24" s="6" t="s">
         <v>107</v>
       </c>
@@ -2047,7 +2053,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" hidden="1">
       <c r="A25" s="11" t="s">
         <v>111</v>
       </c>
@@ -2151,7 +2157,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" hidden="1">
       <c r="A29" s="11" t="s">
         <v>126</v>
       </c>
@@ -2229,7 +2235,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" hidden="1">
       <c r="A32" s="6" t="s">
         <v>140</v>
       </c>
@@ -2307,7 +2313,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" hidden="1">
       <c r="A35" s="39" t="s">
         <v>155</v>
       </c>
@@ -2385,7 +2391,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" hidden="1">
       <c r="A38" s="31" t="s">
         <v>168</v>
       </c>
@@ -2411,7 +2417,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" hidden="1">
       <c r="A39" s="16" t="s">
         <v>173</v>
       </c>
@@ -2437,7 +2443,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" hidden="1">
       <c r="A40" s="31" t="s">
         <v>178</v>
       </c>
@@ -2463,7 +2469,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" hidden="1">
       <c r="A41" s="16" t="s">
         <v>182</v>
       </c>
@@ -2489,7 +2495,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" hidden="1">
       <c r="A42" s="31" t="s">
         <v>185</v>
       </c>
@@ -2541,7 +2547,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" hidden="1">
       <c r="A44" s="31" t="s">
         <v>192</v>
       </c>
@@ -2619,7 +2625,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" hidden="1">
       <c r="A47" s="16" t="s">
         <v>204</v>
       </c>

</xml_diff>